<commit_message>
Update the excel sheets
</commit_message>
<xml_diff>
--- a/metadata/metadata_blank.xlsx
+++ b/metadata/metadata_blank.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="115">
   <si>
     <t>sample_num</t>
   </si>
@@ -35,9 +35,6 @@
     <t>used</t>
   </si>
   <si>
-    <t>If you want to exclude a particular sample from analysis enter "no", otherwise enter "yes"</t>
-  </si>
-  <si>
     <t>sample_short_name</t>
   </si>
   <si>
@@ -242,9 +239,6 @@
     <t>ph</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
     <t>After submission to SRA you can get these numbers.</t>
   </si>
   <si>
@@ -254,9 +248,6 @@
     <t>output_dir</t>
   </si>
   <si>
-    <t>The output directory for this project. All the results from the pipeline as well as the intermediary steps will be placed here</t>
-  </si>
-  <si>
     <t>grouping</t>
   </si>
   <si>
@@ -296,9 +287,6 @@
     <t>Optional metadata</t>
   </si>
   <si>
-    <t>You can add any extra columns  of optional metadata here.</t>
-  </si>
-  <si>
     <t>primer_mismatches</t>
   </si>
   <si>
@@ -308,9 +296,6 @@
     <t>primer_max_dist</t>
   </si>
   <si>
-    <t>How far away from the start of the read can we locate the primer sequence before we discard that read? Enter a value between 0 and 150.</t>
-  </si>
-  <si>
     <t>min_read_len</t>
   </si>
   <si>
@@ -344,12 +329,6 @@
     <t>Mandatory information if you want to submit to SRA (see the "MIxS Compliance" documents).</t>
   </si>
   <si>
-    <t>How short can a read be at a minimum (after primer tunrcation) before we discard that read? No value will disable this check.</t>
-  </si>
-  <si>
-    <t>How long can a read be at a maximum (after primer tunrcation) before we discard that read? No value will disable this check.</t>
-  </si>
-  <si>
     <t>These metadata correspond to SRA required information. See the online NCBI tutorial for more information about these parameters and their definitions.</t>
   </si>
   <si>
@@ -359,10 +338,40 @@
     <t>For all these environemental SRA fields, only certain values are permitted.</t>
   </si>
   <si>
-    <t>You are free to describe the project name with any characters you want. Within the sample project however this field must be identical for all entries.</t>
-  </si>
-  <si>
     <t>This typically represents the version number of the software running on the sequencer.</t>
+  </si>
+  <si>
+    <t>The output directory for this project. All the results from the pipeline as well as the intermediary steps will be placed here.</t>
+  </si>
+  <si>
+    <t>You are free to describe the project name with any characters you want. Within the same project however this field must be identical for all entries.</t>
+  </si>
+  <si>
+    <t>phred_window_size</t>
+  </si>
+  <si>
+    <t>phred_threshold</t>
+  </si>
+  <si>
+    <t>How long can a read be at a maximum (after primer truncation) before we discard that read? No value will disable this check.</t>
+  </si>
+  <si>
+    <t>How short can a read be at a minimum (after primer truncation) before we discard that read? No value will disable this check.</t>
+  </si>
+  <si>
+    <t>How large should the rolling average window be in base pairs when we filter reads based on their quality scores? No value will disable this check.</t>
+  </si>
+  <si>
+    <t>What quality score value should every window have at a minimum before we discard that read? No value will disable this check.</t>
+  </si>
+  <si>
+    <t>How far away from the start of the read can we locate the primer sequence before we discard that read? Enter a value between 0 and 150. No value will disable this check.</t>
+  </si>
+  <si>
+    <t>You can add any extra columns of optional metadata here.</t>
+  </si>
+  <si>
+    <t>If you want to exclude a particular sample from analysis enter "no", otherwise enter "yes".</t>
   </si>
 </sst>
 </file>
@@ -755,10 +764,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BW2"/>
+  <dimension ref="A1:BX2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AN1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="AT1" sqref="AT1"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -834,198 +843,203 @@
     <col min="72" max="72" width="20.5" style="4" customWidth="1"/>
     <col min="73" max="73" width="19.33203125" style="4" customWidth="1"/>
     <col min="74" max="74" width="20.83203125" style="4" customWidth="1"/>
-    <col min="75" max="16384" width="10.83203125" style="4"/>
+    <col min="75" max="75" width="25.1640625" style="4" customWidth="1"/>
+    <col min="76" max="76" width="21.83203125" style="4" customWidth="1"/>
+    <col min="77" max="16384" width="10.83203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:75" s="1" customFormat="1" ht="154" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:76" s="1" customFormat="1" ht="154" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>7</v>
-      </c>
       <c r="E1" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AN1" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AO1" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="AP1" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="AQ1" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="AR1" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="AS1" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="AT1" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="AU1" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="AV1" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="AX1" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="AY1" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="AZ1" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="BA1" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="BC1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="BD1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="BF1" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="BG1" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="BH1" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="BI1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="BJ1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="BK1" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="BM1" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="BO1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="BP1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="BQ1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="BS1" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="BT1" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="BU1" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="BV1" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="BW1" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="AB1" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="AC1" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="AE1" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="AF1" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="AG1" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="AH1" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="AI1" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="AK1" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="AL1" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="AN1" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="AO1" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="AP1" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="AQ1" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="AR1" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="AS1" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="AT1" s="1" t="s">
+      <c r="BX1" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="AU1" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="AV1" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="AX1" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="AY1" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="AZ1" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="BA1" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="BC1" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="BD1" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="BF1" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="BG1" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="BH1" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="BI1" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="BJ1" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="BK1" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="BM1" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="BO1" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="BP1" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="BQ1" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="BS1" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="BT1" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="BU1" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="BV1" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="BW1" s="1" t="s">
-        <v>71</v>
-      </c>
     </row>
-    <row r="2" spans="1:75" s="2" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:76" s="2" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1033,178 +1047,184 @@
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>4</v>
-      </c>
       <c r="E2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>9</v>
-      </c>
       <c r="H2" s="2" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="J2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="K2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="L2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="L2" s="2" t="s">
-        <v>13</v>
-      </c>
       <c r="N2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="O2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="P2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="Q2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="Q2" s="2" t="s">
-        <v>19</v>
-      </c>
       <c r="S2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="T2" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="T2" s="2" t="s">
+      <c r="U2" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="U2" s="2" t="s">
-        <v>27</v>
-      </c>
       <c r="V2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="W2" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="W2" s="2" t="s">
+      <c r="X2" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="X2" s="2" t="s">
-        <v>32</v>
-      </c>
       <c r="Z2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA2" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB2" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="AA2" s="2" t="s">
+      <c r="AC2" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="AB2" s="2" t="s">
+      <c r="AE2" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="AF2" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="AC2" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="AE2" s="2" t="s">
+      <c r="AG2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="AH2" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="AF2" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="AG2" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="AH2" s="2" t="s">
+      <c r="AI2" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="AI2" s="2" t="s">
+      <c r="AK2" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="AL2" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="AK2" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="AL2" s="2" t="s">
-        <v>48</v>
-      </c>
       <c r="AN2" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="AO2" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="AO2" s="2" t="s">
+      <c r="AP2" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="AP2" s="2" t="s">
+      <c r="AQ2" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="AR2" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="AQ2" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="AR2" s="2" t="s">
+      <c r="AS2" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="AS2" s="2" t="s">
+      <c r="AT2" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="AT2" s="2" t="s">
+      <c r="AU2" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="AU2" s="2" t="s">
+      <c r="AV2" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="AV2" s="2" t="s">
+      <c r="AX2" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="AX2" s="2" t="s">
+      <c r="AY2" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="AY2" s="2" t="s">
+      <c r="AZ2" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="AZ2" s="2" t="s">
+      <c r="BA2" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="BA2" s="2" t="s">
+      <c r="BC2" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="BD2" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="BF2" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="BC2" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="BD2" s="2" t="s">
+      <c r="BG2" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="BH2" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="BI2" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="BF2" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="BG2" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="BH2" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="BI2" s="2" t="s">
+      <c r="BJ2" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="BJ2" s="2" t="s">
-        <v>70</v>
-      </c>
       <c r="BM2" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="BO2" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="BP2" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="BO2" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="BP2" s="2" t="s">
+      <c r="BQ2" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="BQ2" s="2" t="s">
-        <v>80</v>
-      </c>
       <c r="BS2" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="BT2" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="BU2" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="BV2" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="BT2" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="BU2" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="BV2" s="2" t="s">
-        <v>95</v>
+      <c r="BW2" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="BX2" s="2" t="s">
+        <v>107</v>
       </c>
     </row>
   </sheetData>

</xml_diff>